<commit_message>
More data model tweaks
</commit_message>
<xml_diff>
--- a/dds/economics.xlsx
+++ b/dds/economics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="526"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="526" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="97">
   <si>
     <t>Identifier</t>
   </si>
@@ -317,6 +317,12 @@
   </si>
   <si>
     <t>Auto Only</t>
+  </si>
+  <si>
+    <t>filter.device_shared</t>
+  </si>
+  <si>
+    <t>cost</t>
   </si>
 </sst>
 </file>
@@ -834,9 +840,9 @@
   </sheetPr>
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C18" sqref="C18"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1673,10 +1679,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1705,6 +1711,17 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add variable 'project.estimate_energy_record' as a flag for calculating energy record from annual energy
</commit_message>
<xml_diff>
--- a/dds/economics.xlsx
+++ b/dds/economics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="526" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="526"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="101">
   <si>
     <t>Identifier</t>
   </si>
@@ -323,19 +323,38 @@
   </si>
   <si>
     <t>cost</t>
+  </si>
+  <si>
+    <t>project.estimate_energy_record</t>
+  </si>
+  <si>
+    <t>Estimate Energy Record</t>
+  </si>
+  <si>
+    <t>Estimate energy record from annual energy if True</t>
+  </si>
+  <si>
+    <t>bool</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -386,13 +405,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -428,43 +447,44 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="40% - Accent2" xfId="2" builtinId="35"/>
-    <cellStyle name="40% - Accent5" xfId="3" builtinId="47"/>
+    <cellStyle name="40% - Accent3" xfId="3" builtinId="39"/>
+    <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -840,9 +860,9 @@
   </sheetPr>
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -884,280 +904,288 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
+    <row r="20" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+    <row r="21" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B22" s="4"/>
@@ -1253,10 +1281,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1432,6 +1460,14 @@
       </c>
       <c r="B20" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1681,7 +1717,7 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Switch from per MW phase cost estimates to absolute values
</commit_message>
<xml_diff>
--- a/dds/economics.xlsx
+++ b/dds/economics.xlsx
@@ -18,6 +18,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="195">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -67,7 +68,7 @@
     <t xml:space="preserve">project.annual_array_mttf_estimate</t>
   </si>
   <si>
-    <t xml:space="preserve">Annual Array MTTF Estimste</t>
+    <t xml:space="preserve">Annual Array MTTF Estimate</t>
   </si>
   <si>
     <t xml:space="preserve">Estimate for the annual mean time to failure of the array</t>
@@ -94,19 +95,19 @@
     <t xml:space="preserve">project.electrical_cost_estimate</t>
   </si>
   <si>
-    <t xml:space="preserve">Electrical Sub-Systems Cost Estimate Per MW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimated costs for the electrical sub-systems per MW of rated installed power</t>
+    <t xml:space="preserve">Electrical Sub-Systems Cost Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated costs for the electrical sub-systems</t>
   </si>
   <si>
     <t xml:space="preserve">project.installation_cost_estimate</t>
   </si>
   <si>
-    <t xml:space="preserve">Installation Cost Estimate Per MW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimated costs for installation of array per MW of rated installed power</t>
+    <t xml:space="preserve">Installation Cost Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated costs for installation of array</t>
   </si>
   <si>
     <t xml:space="preserve">project.lifetime</t>
@@ -118,19 +119,19 @@
     <t xml:space="preserve">project.moorings_cost_estimate</t>
   </si>
   <si>
-    <t xml:space="preserve">Moorings and Foundations Cost Estimate Per MW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimated costs for the moorings and foundations per MW of rated installed power</t>
+    <t xml:space="preserve">Moorings and Foundations Cost Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated costs for the moorings and foundations</t>
   </si>
   <si>
     <t xml:space="preserve">project.opex_estimate</t>
   </si>
   <si>
-    <t xml:space="preserve">Annual OPEX Estimate Per MW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimate for the annual OPEX costs per MW of rated installed power</t>
+    <t xml:space="preserve">Annual OPEX Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimate for the annual OPEX costs</t>
   </si>
   <si>
     <t xml:space="preserve">project.estimate_energy_record</t>
@@ -569,9 +570,6 @@
   </si>
   <si>
     <t xml:space="preserve">Years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Euro/MW</t>
   </si>
   <si>
     <t xml:space="preserve">Euro/year</t>
@@ -663,7 +661,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -672,20 +670,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD7E4BD"/>
-        <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFB9CDE5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFB9CDE5"/>
-        <bgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -714,7 +700,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -741,14 +727,8 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -761,23 +741,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -785,7 +761,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -801,25 +777,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in 40% - Accent3" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in 40% - Accent5" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in 40% - Accent1" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -837,7 +807,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -857,7 +827,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFD7E4BD"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -896,10 +866,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B16" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
-      <selection pane="topRight" activeCell="D48" activeCellId="0" sqref="D48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="C3" activeCellId="0" sqref="C:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -956,866 +926,866 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+    <row r="3" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    <row r="4" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+    <row r="10" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+    <row r="13" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+    <row r="14" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
+    <row r="15" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
       <c r="AMG15" s="0"/>
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
-    <row r="16" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+    <row r="16" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
       <c r="AMJ16" s="0"/>
     </row>
-    <row r="17" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+    <row r="17" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
+    <row r="18" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="B18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row r="19" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+    <row r="19" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
       <c r="AMG19" s="0"/>
       <c r="AMH19" s="0"/>
       <c r="AMI19" s="0"/>
       <c r="AMJ19" s="0"/>
     </row>
-    <row r="20" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
+    <row r="20" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
       <c r="AMG20" s="0"/>
       <c r="AMH20" s="0"/>
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
+    <row r="22" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
       <c r="AMI22" s="0"/>
       <c r="AMJ22" s="0"/>
     </row>
-    <row r="23" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
+    <row r="23" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="B23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>
       <c r="AMI23" s="0"/>
       <c r="AMJ23" s="0"/>
     </row>
-    <row r="24" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
+    <row r="24" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="7" t="s">
+      <c r="B24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
       <c r="AMG24" s="0"/>
       <c r="AMH24" s="0"/>
       <c r="AMI24" s="0"/>
       <c r="AMJ24" s="0"/>
     </row>
-    <row r="25" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="s">
+    <row r="25" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="B25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
       <c r="AMG26" s="0"/>
       <c r="AMH26" s="0"/>
       <c r="AMI26" s="0"/>
       <c r="AMJ26" s="0"/>
     </row>
-    <row r="27" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
+    <row r="27" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="B27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
       <c r="AMG27" s="0"/>
       <c r="AMH27" s="0"/>
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
-    <row r="28" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+    <row r="28" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="B28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
       <c r="AMG28" s="0"/>
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
+    <row r="29" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="7" t="s">
+      <c r="B30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
       <c r="AMG30" s="0"/>
       <c r="AMH30" s="0"/>
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
+    <row r="31" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="7" t="s">
+      <c r="B31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
       <c r="AMG31" s="0"/>
       <c r="AMH31" s="0"/>
       <c r="AMI31" s="0"/>
       <c r="AMJ31" s="0"/>
     </row>
-    <row r="32" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
+    <row r="32" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="7" t="s">
+      <c r="B32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
       <c r="AMG32" s="0"/>
       <c r="AMH32" s="0"/>
       <c r="AMI32" s="0"/>
       <c r="AMJ32" s="0"/>
     </row>
-    <row r="33" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
+    <row r="33" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="B33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-    </row>
-    <row r="34" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="7" t="s">
+      <c r="B34" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
       <c r="AMG34" s="0"/>
       <c r="AMH34" s="0"/>
       <c r="AMI34" s="0"/>
       <c r="AMJ34" s="0"/>
     </row>
-    <row r="35" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
+    <row r="35" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="7" t="s">
+      <c r="B35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
       <c r="AMG35" s="0"/>
       <c r="AMH35" s="0"/>
       <c r="AMI35" s="0"/>
       <c r="AMJ35" s="0"/>
     </row>
-    <row r="36" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
+    <row r="36" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="7" t="s">
+      <c r="B36" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
       <c r="AMG36" s="0"/>
       <c r="AMH36" s="0"/>
       <c r="AMI36" s="0"/>
       <c r="AMJ36" s="0"/>
     </row>
-    <row r="37" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
+    <row r="37" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="7" t="s">
+      <c r="B37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="7" t="s">
+      <c r="B38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
       <c r="AMG38" s="0"/>
       <c r="AMH38" s="0"/>
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
     </row>
-    <row r="39" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
+    <row r="39" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="7" t="s">
+      <c r="B39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
       <c r="AMG39" s="0"/>
       <c r="AMH39" s="0"/>
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
     </row>
-    <row r="40" s="8" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
+    <row r="40" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="7" t="s">
+      <c r="B40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
       <c r="AMG40" s="0"/>
       <c r="AMH40" s="0"/>
       <c r="AMI40" s="0"/>
       <c r="AMJ40" s="0"/>
     </row>
-    <row r="41" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="s">
+    <row r="41" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="B41" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="42" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="B42" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-    </row>
-    <row r="43" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="s">
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="44" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
+    <row r="44" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="45" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
+    <row r="45" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="46" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="9" t="s">
+    <row r="46" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B46" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="9" t="s">
+      <c r="B46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="47" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="9" t="s">
+    <row r="47" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B47" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="9" t="s">
+      <c r="B47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="8" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="48" s="6" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6" t="s">
+    <row r="48" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="5" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1841,38 +1811,38 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C:D A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="18.18"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1933,7 +1903,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+      <selection pane="topLeft" activeCell="A47" activeCellId="1" sqref="C:D A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1943,19 +1913,19 @@
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>170</v>
       </c>
     </row>
@@ -1963,7 +1933,7 @@
       <c r="A2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2008,7 +1978,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -2016,7 +1986,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -2024,7 +1994,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -2322,7 +2292,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="7" t="s">
         <v>142</v>
       </c>
       <c r="B45" s="0" t="s">
@@ -2330,7 +2300,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B46" s="0" t="s">
@@ -2338,7 +2308,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="12" t="s">
         <v>148</v>
       </c>
       <c r="B47" s="0" t="s">
@@ -2364,10 +2334,10 @@
   </sheetPr>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B22" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="topRight" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B16" activeCellId="1" sqref="C:D B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2377,19 +2347,19 @@
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2414,7 +2384,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2422,7 +2392,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,31 +2400,31 @@
         <v>23</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="0" t="s">
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,13 +2432,13 @@
         <v>37</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>178</v>
@@ -2477,10 +2447,10 @@
         <v>178</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,7 +2458,7 @@
         <v>41</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,7 +2466,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2504,7 +2474,7 @@
         <v>47</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2512,7 +2482,7 @@
         <v>50</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,7 +2490,7 @@
         <v>53</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,7 +2498,7 @@
         <v>56</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2536,7 +2506,7 @@
         <v>59</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2544,7 +2514,7 @@
         <v>62</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2552,7 +2522,7 @@
         <v>65</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2560,7 +2530,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2568,7 +2538,7 @@
         <v>71</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2576,7 +2546,7 @@
         <v>74</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2648,7 +2618,7 @@
         <v>101</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2656,7 +2626,7 @@
         <v>104</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,7 +2634,7 @@
         <v>107</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2672,7 +2642,7 @@
         <v>110</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2680,7 +2650,7 @@
         <v>113</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2688,7 +2658,7 @@
         <v>116</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,7 +2666,7 @@
         <v>119</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2704,7 +2674,7 @@
         <v>122</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2744,14 +2714,14 @@
         <v>138</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="7" t="s">
         <v>142</v>
       </c>
       <c r="B44" s="0" t="s">
@@ -2759,7 +2729,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B45" s="0" t="s">
@@ -2767,7 +2737,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="12" t="s">
         <v>148</v>
       </c>
       <c r="B46" s="0" t="s">
@@ -2794,7 +2764,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C:D B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2806,20 +2776,20 @@
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>188</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>189</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
@@ -2830,10 +2800,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>190</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2856,7 +2826,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="C:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2866,20 +2836,20 @@
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add breakdowns of CAPEX and OPEX LCOE values
</commit_message>
<xml_diff>
--- a/dds/economics.xlsx
+++ b/dds/economics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,7 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="202">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -485,6 +486,24 @@
     <t xml:space="preserve">Most likely OPEX cost breakdown</t>
   </si>
   <si>
+    <t xml:space="preserve">project.capex_lcoe_breakdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most Likely CAPEX LCOE Breakdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPEX cost breakdown per most likely discounted energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project.opex_lcoe_breakdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most Likely OPEX LCOE Breakdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEX cost breakdown per most likely discounted energy</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
@@ -585,6 +604,9 @@
   </si>
   <si>
     <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cent/kWh</t>
   </si>
   <si>
     <t xml:space="preserve">Table 1</t>
@@ -864,12 +886,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ48"/>
+  <dimension ref="A1:AMJ50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C3" activeCellId="0" sqref="C:D"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B16" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topRight" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1787,6 +1809,34 @@
       </c>
       <c r="D48" s="5" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="49" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1811,39 +1861,39 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C:D A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="18.18"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,25 +1901,25 @@
         <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1877,10 +1927,10 @@
         <v>138</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1900,10 +1950,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A47" activeCellId="1" sqref="C:D A47"/>
+      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1914,19 +1964,19 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,7 +1984,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1942,7 +1992,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1950,7 +2000,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1958,7 +2008,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1966,7 +2016,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,7 +2024,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,7 +2032,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,7 +2040,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1998,7 +2048,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,7 +2056,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,25 +2064,25 @@
         <v>37</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2040,7 +2090,7 @@
         <v>41</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2048,7 +2098,7 @@
         <v>44</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,7 +2106,7 @@
         <v>47</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2064,7 +2114,7 @@
         <v>50</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2072,7 +2122,7 @@
         <v>53</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,7 +2130,7 @@
         <v>56</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,7 +2138,7 @@
         <v>59</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2096,7 +2146,7 @@
         <v>62</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,7 +2154,7 @@
         <v>65</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2112,7 +2162,7 @@
         <v>68</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2120,7 +2170,7 @@
         <v>71</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2128,7 +2178,7 @@
         <v>74</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2136,7 +2186,7 @@
         <v>77</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,7 +2194,7 @@
         <v>80</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2202,7 @@
         <v>83</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,7 +2210,7 @@
         <v>86</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2168,7 +2218,7 @@
         <v>89</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,7 +2226,7 @@
         <v>92</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2184,7 +2234,7 @@
         <v>95</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,7 +2242,7 @@
         <v>98</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2200,7 +2250,7 @@
         <v>101</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2208,7 +2258,7 @@
         <v>104</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2216,7 +2266,7 @@
         <v>107</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,7 +2274,7 @@
         <v>110</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,7 +2282,7 @@
         <v>113</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2240,7 +2290,7 @@
         <v>116</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2248,7 +2298,7 @@
         <v>119</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,7 +2306,7 @@
         <v>122</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,7 +2314,7 @@
         <v>125</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2272,7 +2322,7 @@
         <v>128</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2280,7 +2330,7 @@
         <v>131</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2288,7 +2338,7 @@
         <v>135</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2296,7 +2346,7 @@
         <v>142</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2304,7 +2354,7 @@
         <v>145</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2312,7 +2362,23 @@
         <v>148</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2332,12 +2398,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B16" activeCellId="1" sqref="C:D B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B16" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topRight" activeCell="B51" activeCellId="0" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2348,19 +2414,19 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2368,7 +2434,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,7 +2442,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2384,7 +2450,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2392,7 +2458,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,7 +2466,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2408,7 +2474,7 @@
         <v>31</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2416,7 +2482,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2424,7 +2490,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,25 +2498,25 @@
         <v>37</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2458,7 +2524,7 @@
         <v>41</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,7 +2532,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,7 +2540,7 @@
         <v>47</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2482,7 +2548,7 @@
         <v>50</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2490,7 +2556,7 @@
         <v>53</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2498,7 +2564,7 @@
         <v>56</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,7 +2572,7 @@
         <v>59</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2514,7 +2580,7 @@
         <v>62</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2522,7 +2588,7 @@
         <v>65</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2530,7 +2596,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2538,7 +2604,7 @@
         <v>71</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,7 +2612,7 @@
         <v>74</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2554,7 +2620,7 @@
         <v>77</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2562,7 +2628,7 @@
         <v>80</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2570,7 +2636,7 @@
         <v>83</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2578,7 +2644,7 @@
         <v>86</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2586,7 +2652,7 @@
         <v>89</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,7 +2660,7 @@
         <v>92</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2602,7 +2668,7 @@
         <v>95</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2610,7 +2676,7 @@
         <v>98</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2618,7 +2684,7 @@
         <v>101</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2626,7 +2692,7 @@
         <v>104</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2634,7 +2700,7 @@
         <v>107</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2642,7 +2708,7 @@
         <v>110</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2650,7 +2716,7 @@
         <v>113</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2658,7 +2724,7 @@
         <v>116</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2666,7 +2732,7 @@
         <v>119</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2674,7 +2740,7 @@
         <v>122</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2682,7 +2748,7 @@
         <v>125</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2690,7 +2756,7 @@
         <v>128</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2698,7 +2764,7 @@
         <v>131</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2706,7 +2772,7 @@
         <v>135</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2714,10 +2780,10 @@
         <v>138</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2725,7 +2791,7 @@
         <v>142</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2733,7 +2799,7 @@
         <v>145</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2741,7 +2807,23 @@
         <v>148</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2764,7 +2846,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C:D B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2777,19 +2859,19 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
@@ -2800,10 +2882,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2826,7 +2908,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="C:D"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2837,19 +2919,19 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix connection between device cost and the database
</commit_message>
<xml_diff>
--- a/dds/economics.xlsx
+++ b/dds/economics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,6 +20,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="204">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -60,13 +61,19 @@
     <t xml:space="preserve">device.system_cost</t>
   </si>
   <si>
+    <t xml:space="preserve">SimpleDataColumn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hidden.device_filtered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project.annual_array_mttf_estimate</t>
+  </si>
+  <si>
     <t xml:space="preserve">SimpleData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Device Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project.annual_array_mttf_estimate</t>
   </si>
   <si>
     <t xml:space="preserve">Annual Array MTTF Estimate</t>
@@ -697,7 +704,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -709,6 +716,13 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -750,7 +764,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -767,15 +785,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -787,8 +821,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -796,6 +834,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -888,956 +930,1015 @@
   </sheetPr>
   <dimension ref="A1:AMJ50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B16" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
-      <selection pane="topRight" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="71.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="9" style="0" width="20.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="110.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="B12" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="C12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="D12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="B13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="D13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="AMG14" s="0"/>
-      <c r="AMH14" s="0"/>
-      <c r="AMI14" s="0"/>
-      <c r="AMJ14" s="0"/>
-    </row>
-    <row r="15" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="B14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="D14" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="AMG14" s="1"/>
+      <c r="AMH14" s="1"/>
+      <c r="AMI14" s="1"/>
+      <c r="AMJ14" s="1"/>
+    </row>
+    <row r="15" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="AMG15" s="0"/>
-      <c r="AMH15" s="0"/>
-      <c r="AMI15" s="0"/>
-      <c r="AMJ15" s="0"/>
-    </row>
-    <row r="16" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="B15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="D15" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="AMG15" s="1"/>
+      <c r="AMH15" s="1"/>
+      <c r="AMI15" s="1"/>
+      <c r="AMJ15" s="1"/>
+    </row>
+    <row r="16" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="AMG16" s="0"/>
-      <c r="AMH16" s="0"/>
-      <c r="AMI16" s="0"/>
-      <c r="AMJ16" s="0"/>
-    </row>
-    <row r="17" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="B16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="D16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="AMG16" s="1"/>
+      <c r="AMH16" s="1"/>
+      <c r="AMI16" s="1"/>
+      <c r="AMJ16" s="1"/>
+    </row>
+    <row r="17" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="B17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="D17" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="AMG18" s="0"/>
-      <c r="AMH18" s="0"/>
-      <c r="AMI18" s="0"/>
-      <c r="AMJ18" s="0"/>
-    </row>
-    <row r="19" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="B18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="D18" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="AMG18" s="1"/>
+      <c r="AMH18" s="1"/>
+      <c r="AMI18" s="1"/>
+      <c r="AMJ18" s="1"/>
+    </row>
+    <row r="19" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="AMG19" s="0"/>
-      <c r="AMH19" s="0"/>
-      <c r="AMI19" s="0"/>
-      <c r="AMJ19" s="0"/>
-    </row>
-    <row r="20" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="B19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="D19" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="AMG19" s="1"/>
+      <c r="AMH19" s="1"/>
+      <c r="AMI19" s="1"/>
+      <c r="AMJ19" s="1"/>
+    </row>
+    <row r="20" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="AMG20" s="0"/>
-      <c r="AMH20" s="0"/>
-      <c r="AMI20" s="0"/>
-      <c r="AMJ20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="B20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="D20" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="AMG20" s="1"/>
+      <c r="AMH20" s="1"/>
+      <c r="AMI20" s="1"/>
+      <c r="AMJ20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="22" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
+      <c r="B21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="D21" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="AMG22" s="0"/>
-      <c r="AMH22" s="0"/>
-      <c r="AMI22" s="0"/>
-      <c r="AMJ22" s="0"/>
-    </row>
-    <row r="23" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="B22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="D22" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="AMG22" s="1"/>
+      <c r="AMH22" s="1"/>
+      <c r="AMI22" s="1"/>
+      <c r="AMJ22" s="1"/>
+    </row>
+    <row r="23" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="AMG23" s="0"/>
-      <c r="AMH23" s="0"/>
-      <c r="AMI23" s="0"/>
-      <c r="AMJ23" s="0"/>
-    </row>
-    <row r="24" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="B23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="D23" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="AMG23" s="1"/>
+      <c r="AMH23" s="1"/>
+      <c r="AMI23" s="1"/>
+      <c r="AMJ23" s="1"/>
+    </row>
+    <row r="24" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="AMG24" s="0"/>
-      <c r="AMH24" s="0"/>
-      <c r="AMI24" s="0"/>
-      <c r="AMJ24" s="0"/>
-    </row>
-    <row r="25" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="B24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="D24" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="AMG24" s="1"/>
+      <c r="AMH24" s="1"/>
+      <c r="AMI24" s="1"/>
+      <c r="AMJ24" s="1"/>
+    </row>
+    <row r="25" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
+      <c r="B25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="D25" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="AMG26" s="0"/>
-      <c r="AMH26" s="0"/>
-      <c r="AMI26" s="0"/>
-      <c r="AMJ26" s="0"/>
-    </row>
-    <row r="27" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
+      <c r="B26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="D26" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="AMG26" s="1"/>
+      <c r="AMH26" s="1"/>
+      <c r="AMI26" s="1"/>
+      <c r="AMJ26" s="1"/>
+    </row>
+    <row r="27" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="AMG27" s="0"/>
-      <c r="AMH27" s="0"/>
-      <c r="AMI27" s="0"/>
-      <c r="AMJ27" s="0"/>
-    </row>
-    <row r="28" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
+      <c r="B27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="D27" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="AMG27" s="1"/>
+      <c r="AMH27" s="1"/>
+      <c r="AMI27" s="1"/>
+      <c r="AMJ27" s="1"/>
+    </row>
+    <row r="28" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="AMG28" s="0"/>
-      <c r="AMH28" s="0"/>
-      <c r="AMI28" s="0"/>
-      <c r="AMJ28" s="0"/>
-    </row>
-    <row r="29" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
+      <c r="B28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="D28" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="AMG28" s="1"/>
+      <c r="AMH28" s="1"/>
+      <c r="AMI28" s="1"/>
+      <c r="AMJ28" s="1"/>
+    </row>
+    <row r="29" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
+      <c r="B29" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="D29" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="AMG30" s="0"/>
-      <c r="AMH30" s="0"/>
-      <c r="AMI30" s="0"/>
-      <c r="AMJ30" s="0"/>
-    </row>
-    <row r="31" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
+      <c r="B30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="D30" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="AMG30" s="1"/>
+      <c r="AMH30" s="1"/>
+      <c r="AMI30" s="1"/>
+      <c r="AMJ30" s="1"/>
+    </row>
+    <row r="31" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="AMG31" s="0"/>
-      <c r="AMH31" s="0"/>
-      <c r="AMI31" s="0"/>
-      <c r="AMJ31" s="0"/>
-    </row>
-    <row r="32" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="s">
+      <c r="B31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="6" t="s">
+      <c r="D31" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="AMG31" s="1"/>
+      <c r="AMH31" s="1"/>
+      <c r="AMI31" s="1"/>
+      <c r="AMJ31" s="1"/>
+    </row>
+    <row r="32" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="AMG32" s="0"/>
-      <c r="AMH32" s="0"/>
-      <c r="AMI32" s="0"/>
-      <c r="AMJ32" s="0"/>
-    </row>
-    <row r="33" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
+      <c r="B32" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="D32" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="AMG32" s="1"/>
+      <c r="AMH32" s="1"/>
+      <c r="AMI32" s="1"/>
+      <c r="AMJ32" s="1"/>
+    </row>
+    <row r="33" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
+      <c r="B33" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="D33" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+    </row>
+    <row r="34" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="AMG34" s="0"/>
-      <c r="AMH34" s="0"/>
-      <c r="AMI34" s="0"/>
-      <c r="AMJ34" s="0"/>
-    </row>
-    <row r="35" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
+      <c r="B34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="D34" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="AMG34" s="1"/>
+      <c r="AMH34" s="1"/>
+      <c r="AMI34" s="1"/>
+      <c r="AMJ34" s="1"/>
+    </row>
+    <row r="35" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="AMG35" s="0"/>
-      <c r="AMH35" s="0"/>
-      <c r="AMI35" s="0"/>
-      <c r="AMJ35" s="0"/>
-    </row>
-    <row r="36" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="s">
+      <c r="B35" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="D35" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="AMG35" s="1"/>
+      <c r="AMH35" s="1"/>
+      <c r="AMI35" s="1"/>
+      <c r="AMJ35" s="1"/>
+    </row>
+    <row r="36" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="AMG36" s="0"/>
-      <c r="AMH36" s="0"/>
-      <c r="AMI36" s="0"/>
-      <c r="AMJ36" s="0"/>
-    </row>
-    <row r="37" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
+      <c r="B36" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="6" t="s">
+      <c r="D36" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="AMG36" s="1"/>
+      <c r="AMH36" s="1"/>
+      <c r="AMI36" s="1"/>
+      <c r="AMJ36" s="1"/>
+    </row>
+    <row r="37" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-    </row>
-    <row r="38" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6" t="s">
+      <c r="B37" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="6" t="s">
+      <c r="D37" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="AMG38" s="0"/>
-      <c r="AMH38" s="0"/>
-      <c r="AMI38" s="0"/>
-      <c r="AMJ38" s="0"/>
-    </row>
-    <row r="39" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
+      <c r="B38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="6" t="s">
+      <c r="D38" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="AMG38" s="1"/>
+      <c r="AMH38" s="1"/>
+      <c r="AMI38" s="1"/>
+      <c r="AMJ38" s="1"/>
+    </row>
+    <row r="39" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="AMG39" s="0"/>
-      <c r="AMH39" s="0"/>
-      <c r="AMI39" s="0"/>
-      <c r="AMJ39" s="0"/>
-    </row>
-    <row r="40" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="s">
+      <c r="B39" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="6" t="s">
+      <c r="D39" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="AMG39" s="1"/>
+      <c r="AMH39" s="1"/>
+      <c r="AMI39" s="1"/>
+      <c r="AMJ39" s="1"/>
+    </row>
+    <row r="40" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="AMG40" s="0"/>
-      <c r="AMH40" s="0"/>
-      <c r="AMI40" s="0"/>
-      <c r="AMJ40" s="0"/>
-    </row>
-    <row r="41" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
+      <c r="B40" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="D40" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="AMG40" s="1"/>
+      <c r="AMH40" s="1"/>
+      <c r="AMI40" s="1"/>
+      <c r="AMJ40" s="1"/>
+    </row>
+    <row r="41" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" s="3" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
+      <c r="B41" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="5" t="s">
+      <c r="D41" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
+      <c r="B42" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="D42" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="43" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="B43" s="9" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="44" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
+      <c r="C43" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="D43" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="9" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="45" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6" t="s">
+      <c r="B44" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="D44" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+    </row>
+    <row r="45" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="B45" s="9" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="46" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="s">
+      <c r="C45" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="8" t="s">
+      <c r="D45" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+    </row>
+    <row r="46" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="13" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="47" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
+      <c r="B46" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="8" t="s">
+      <c r="D46" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+    </row>
+    <row r="47" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="13" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="48" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
+      <c r="B47" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="5" t="s">
+      <c r="D47" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+    </row>
+    <row r="48" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="9" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="49" s="5" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
+      <c r="B48" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C49" s="5" t="s">
+      <c r="D48" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+    </row>
+    <row r="49" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="9" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="50" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
+      <c r="B49" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C50" s="5" t="s">
+      <c r="D49" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+    </row>
+    <row r="50" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="9" t="s">
         <v>156</v>
       </c>
+      <c r="B50" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H11"/>
@@ -1870,67 +1971,67 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="18.18"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="9" t="s">
+    <row r="1" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="D1" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="F1" s="14" t="s">
         <v>164</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1962,29 +2063,29 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="20.37"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="D1" s="9" t="s">
+    <row r="1" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="14" t="s">
         <v>176</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>177</v>
+        <v>19</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,393 +2093,393 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>31</v>
+      <c r="A8" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>14</v>
+      <c r="A9" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>11</v>
+      <c r="A10" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
-        <v>142</v>
+      <c r="A45" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
-        <v>145</v>
+      <c r="A46" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12" t="s">
-        <v>148</v>
+      <c r="A47" s="19" t="s">
+        <v>150</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="12" t="s">
-        <v>151</v>
+      <c r="A48" s="19" t="s">
+        <v>153</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="12" t="s">
-        <v>154</v>
+      <c r="A49" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2400,7 +2501,7 @@
   </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B16" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
       <selection pane="topRight" activeCell="B51" activeCellId="0" sqref="B51"/>
@@ -2412,21 +2513,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="20.37"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="D1" s="9" t="s">
+    <row r="1" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="14" t="s">
         <v>183</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,396 +2535,396 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>31</v>
+      <c r="A7" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>14</v>
+      <c r="A8" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>11</v>
+      <c r="A9" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="s">
-        <v>142</v>
+      <c r="A44" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
-        <v>145</v>
+      <c r="A45" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="12" t="s">
-        <v>148</v>
+      <c r="A46" s="19" t="s">
+        <v>150</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12" t="s">
-        <v>151</v>
+      <c r="A47" s="19" t="s">
+        <v>153</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="12" t="s">
-        <v>154</v>
+      <c r="A48" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2857,23 +2958,23 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="20.37"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="D1" s="9" t="s">
+    <row r="1" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2882,10 +2983,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2917,21 +3018,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="20.37"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="D1" s="9" t="s">
+    <row r="1" s="15" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="14" t="s">
         <v>201</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add CAPEX vs OPEX comparison for most likely LCOE
</commit_message>
<xml_diff>
--- a/dds/economics.xlsx
+++ b/dds/economics.xlsx
@@ -26,6 +26,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="168">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -358,6 +359,15 @@
   </si>
   <si>
     <t xml:space="preserve">Discounted OPEX cost breakdown for the most likely LCOE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project.lcoe_breakdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most Likely LCOE Breakdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPEX vs OPEX contributions to the most likely LCOE</t>
   </si>
   <si>
     <t xml:space="preserve">project.capex_lcoe_breakdown</t>
@@ -843,7 +853,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topRight" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1505,37 +1515,55 @@
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
+    <row r="36" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="9" t="s">
+      <c r="B36" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="37" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="s">
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="D37" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D37" s="8" t="s">
+    </row>
+    <row r="38" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
+      <c r="B38" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1571,28 +1599,28 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,36 +1628,36 @@
         <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1653,7 +1681,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1664,19 +1692,19 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1684,7 +1712,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,7 +1720,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1700,7 +1728,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,7 +1736,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1716,7 +1744,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,7 +1752,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,7 +1760,7 @@
         <v>33</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,7 +1768,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,7 +1776,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1756,7 +1784,7 @@
         <v>36</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,25 +1792,25 @@
         <v>45</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,7 +1818,7 @@
         <v>49</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1798,7 +1826,7 @@
         <v>58</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,7 +1834,7 @@
         <v>61</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,7 +1842,7 @@
         <v>64</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,7 +1850,7 @@
         <v>67</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,7 +1858,7 @@
         <v>70</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,7 +1866,7 @@
         <v>73</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +1874,7 @@
         <v>76</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,7 +1882,7 @@
         <v>79</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,7 +1890,7 @@
         <v>82</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1870,7 +1898,7 @@
         <v>85</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1906,7 @@
         <v>88</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,7 +1914,7 @@
         <v>91</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +1922,7 @@
         <v>94</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,7 +1930,7 @@
         <v>97</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,7 +1938,7 @@
         <v>101</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1918,7 +1946,7 @@
         <v>39</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,7 +1954,7 @@
         <v>42</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,23 +1962,23 @@
         <v>104</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1958,7 +1986,7 @@
         <v>52</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1966,15 +1994,23 @@
         <v>55</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2016,7 +2052,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B32" activeCellId="0" sqref="B32"/>
+      <selection pane="topRight" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2027,19 +2063,19 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,7 +2083,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2055,7 +2091,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2063,7 +2099,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2071,7 +2107,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,7 +2115,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2087,7 +2123,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2095,7 +2131,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2103,7 +2139,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2111,25 +2147,25 @@
         <v>45</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2137,7 +2173,7 @@
         <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2145,7 +2181,7 @@
         <v>58</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2153,7 +2189,7 @@
         <v>61</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2161,7 +2197,7 @@
         <v>64</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,7 +2205,7 @@
         <v>67</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2177,7 +2213,7 @@
         <v>70</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,7 +2221,7 @@
         <v>73</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,7 +2229,7 @@
         <v>76</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2201,7 +2237,7 @@
         <v>79</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2209,7 +2245,7 @@
         <v>82</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2217,7 +2253,7 @@
         <v>85</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,7 +2261,7 @@
         <v>88</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,7 +2269,7 @@
         <v>91</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2241,7 +2277,7 @@
         <v>94</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2249,7 +2285,7 @@
         <v>97</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2257,7 +2293,7 @@
         <v>101</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2265,7 +2301,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2273,7 +2309,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,37 +2317,37 @@
         <v>104</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="15" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,7 +2355,7 @@
         <v>52</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2327,7 +2363,15 @@
         <v>55</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2380,19 +2424,19 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
@@ -2403,10 +2447,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2440,19 +2484,19 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix economics metrics table units
</commit_message>
<xml_diff>
--- a/dds/economics.xlsx
+++ b/dds/economics.xlsx
@@ -27,6 +27,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">ROOT!$A$1:$H$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2052,7 +2053,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C35" activeCellId="0" sqref="C35"/>
+      <selection pane="topRight" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2142,7 +2143,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>45</v>
       </c>
@@ -2159,16 +2160,16 @@
         <v>149</v>
       </c>
       <c r="F10" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>154</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Allow calculation of some LCOE variables (added median) in less than 3 data points available
</commit_message>
<xml_diff>
--- a/dds/economics.xlsx
+++ b/dds/economics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0B9AC4-2805-4B92-AEB4-8A0736CC0A19}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEB7A29-1B09-4A1D-8526-37C0F7C8455E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="174">
   <si>
     <t>Identifier</t>
   </si>
@@ -339,9 +339,6 @@
     <t>Most Likely Discounted Cost Breakdown</t>
   </si>
   <si>
-    <t>Discounted CAPEX vs OPEX cost breakdown for most likely LCOE</t>
-  </si>
-  <si>
     <t>project.capex_breakdown</t>
   </si>
   <si>
@@ -357,34 +354,22 @@
     <t>Most Likely Discounted OPEX Cost Breakdown</t>
   </si>
   <si>
-    <t>Discounted OPEX cost breakdown for the most likely LCOE</t>
-  </si>
-  <si>
     <t>project.lcoe_breakdown</t>
   </si>
   <si>
     <t>Most Likely LCOE Breakdown</t>
   </si>
   <si>
-    <t>CAPEX vs OPEX contributions to the most likely LCOE</t>
-  </si>
-  <si>
     <t>project.capex_lcoe_breakdown</t>
   </si>
   <si>
     <t>Most Likely CAPEX LCOE Breakdown</t>
   </si>
   <si>
-    <t>CAPEX cost breakdown per discounted energy of most likely LCOE</t>
-  </si>
-  <si>
     <t>project.opex_lcoe_breakdown</t>
   </si>
   <si>
     <t>Most Likely OPEX LCOE Breakdown</t>
-  </si>
-  <si>
-    <t>OPEX cost breakdown per discounted energy of most likely LCOE</t>
   </si>
   <si>
     <t>project.confidence_density</t>
@@ -586,6 +571,30 @@
   </si>
   <si>
     <t>Most likely discounted energy from the combination of discounted OPEX and energy used to determine the most likely LCOE.</t>
+  </si>
+  <si>
+    <t>project.lcoe_median</t>
+  </si>
+  <si>
+    <t>Median Levelised Cost of Energy</t>
+  </si>
+  <si>
+    <t>Median levelised cost of energy in Euro/kWh</t>
+  </si>
+  <si>
+    <t>Discounted CAPEX vs OPEX cost breakdown for most likely or mean LCOE if most likely unavailable</t>
+  </si>
+  <si>
+    <t>Discounted OPEX cost breakdown for the most likely or mean LCOE if most likely unavailable</t>
+  </si>
+  <si>
+    <t>CAPEX vs OPEX contributions to the most likely or mean LCOE if most likely unavailable</t>
+  </si>
+  <si>
+    <t>CAPEX cost breakdown per discounted energy of most likely or mean LCOE if most likely unavailable</t>
+  </si>
+  <si>
+    <t>OPEX cost breakdown per discounted energy of most likely or mean LCOE if most likely unavailable</t>
   </si>
 </sst>
 </file>
@@ -691,7 +700,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -715,6 +724,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1101,11 +1112,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D17" sqref="C2:D39"/>
+      <selection pane="topRight" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,36 +1412,32 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="B17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="D17" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1438,35 +1445,35 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="A18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -1475,16 +1482,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -1493,34 +1500,34 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+        <v>64</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -1529,16 +1536,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1547,16 +1554,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -1565,16 +1572,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1583,16 +1590,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -1601,16 +1608,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -1619,16 +1626,16 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1637,16 +1644,16 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -1655,16 +1662,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>166</v>
+        <v>89</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1673,16 +1680,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>92</v>
+        <v>161</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>94</v>
+        <v>163</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -1691,16 +1698,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -1709,16 +1716,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>101</v>
+        <v>169</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -1727,16 +1734,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -1745,16 +1752,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -1763,16 +1770,16 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>110</v>
+        <v>171</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -1781,57 +1788,75 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>113</v>
+        <v>172</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+    </row>
+    <row r="39" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="8" t="s">
+      <c r="D40" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -1859,28 +1884,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>123</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1888,36 +1913,36 @@
         <v>45</v>
       </c>
       <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" t="s">
         <v>129</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>130</v>
-      </c>
-      <c r="D2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1931,10 +1956,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,19 +1970,19 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1965,7 +1990,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1973,7 +1998,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1981,7 +2006,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1989,7 +2014,7 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1997,7 +2022,7 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2005,7 +2030,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2013,7 +2038,7 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2021,7 +2046,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2029,7 +2054,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2037,7 +2062,7 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2045,25 +2070,25 @@
         <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2071,7 +2096,7 @@
         <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2079,7 +2104,7 @@
         <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2087,7 +2112,7 @@
         <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2095,7 +2120,7 @@
         <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2103,7 +2128,7 @@
         <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2111,7 +2136,7 @@
         <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2119,7 +2144,7 @@
         <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2127,7 +2152,7 @@
         <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2135,7 +2160,7 @@
         <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2143,7 +2168,7 @@
         <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2151,7 +2176,7 @@
         <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2159,7 +2184,7 @@
         <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2167,15 +2192,15 @@
         <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2183,7 +2208,7 @@
         <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2191,15 +2216,15 @@
         <v>95</v>
       </c>
       <c r="B28" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B29" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2207,7 +2232,7 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2215,31 +2240,31 @@
         <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2247,7 +2272,7 @@
         <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2255,23 +2280,31 @@
         <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B38" t="s">
-        <v>140</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2285,11 +2318,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A24" sqref="A24"/>
+      <selection pane="topRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,19 +2333,19 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2320,7 +2353,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2328,7 +2361,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2336,7 +2369,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2344,7 +2377,7 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2352,7 +2385,7 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2360,7 +2393,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2368,7 +2401,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2376,7 +2409,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2384,25 +2417,25 @@
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" t="s">
         <v>147</v>
       </c>
-      <c r="F10" t="s">
-        <v>152</v>
-      </c>
       <c r="G10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" t="s">
         <v>147</v>
-      </c>
-      <c r="H10" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2410,7 +2443,7 @@
         <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2418,7 +2451,7 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2426,7 +2459,7 @@
         <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2434,7 +2467,7 @@
         <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2442,7 +2475,7 @@
         <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2450,7 +2483,7 @@
         <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2458,7 +2491,7 @@
         <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2466,7 +2499,7 @@
         <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2474,7 +2507,7 @@
         <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2482,7 +2515,7 @@
         <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2490,7 +2523,7 @@
         <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2498,7 +2531,7 @@
         <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2506,15 +2539,15 @@
         <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B24" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2522,7 +2555,7 @@
         <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2530,15 +2563,15 @@
         <v>95</v>
       </c>
       <c r="B26" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2546,7 +2579,7 @@
         <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2554,45 +2587,45 @@
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C33" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D33" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2600,7 +2633,7 @@
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2608,15 +2641,23 @@
         <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>153</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>166</v>
+      </c>
+      <c r="B37" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2646,19 +2687,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
@@ -2669,10 +2710,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2700,19 +2741,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add lifetime total cost variables are remove median calculations
</commit_message>
<xml_diff>
--- a/dds/economics.xlsx
+++ b/dds/economics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEB7A29-1B09-4A1D-8526-37C0F7C8455E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65C8D6E-B4CC-4F16-8C2D-757F47B21DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="183">
   <si>
     <t>Identifier</t>
   </si>
@@ -573,15 +573,6 @@
     <t>Most likely discounted energy from the combination of discounted OPEX and energy used to determine the most likely LCOE.</t>
   </si>
   <si>
-    <t>project.lcoe_median</t>
-  </si>
-  <si>
-    <t>Median Levelised Cost of Energy</t>
-  </si>
-  <si>
-    <t>Median levelised cost of energy in Euro/kWh</t>
-  </si>
-  <si>
     <t>Discounted CAPEX vs OPEX cost breakdown for most likely or mean LCOE if most likely unavailable</t>
   </si>
   <si>
@@ -595,6 +586,42 @@
   </si>
   <si>
     <t>OPEX cost breakdown per discounted energy of most likely or mean LCOE if most likely unavailable</t>
+  </si>
+  <si>
+    <t>project.lifetime_cost_mean</t>
+  </si>
+  <si>
+    <t>project.lifetime_cost_mode</t>
+  </si>
+  <si>
+    <t>Mean Lifetime Cost</t>
+  </si>
+  <si>
+    <t>Most Likely Lifetime Cost</t>
+  </si>
+  <si>
+    <t>Mean expenditure for the lifetime of the project</t>
+  </si>
+  <si>
+    <t>Most likely expenditure for the lifetime of the project</t>
+  </si>
+  <si>
+    <t>Mean Discounted Lifetime Cost</t>
+  </si>
+  <si>
+    <t>Most Likely Discounted Lifetime Cost</t>
+  </si>
+  <si>
+    <t>Most likely discounted expenditure for the lifetime of the project</t>
+  </si>
+  <si>
+    <t>Mean discounted expenditure for the lifetime of the project</t>
+  </si>
+  <si>
+    <t>project.discounted_lifetime_cost_mean</t>
+  </si>
+  <si>
+    <t>project.discounted_lifetime_cost_mode</t>
   </si>
 </sst>
 </file>
@@ -725,7 +752,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1112,11 +1139,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D38" sqref="D38"/>
+      <selection pane="topRight" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,32 +1439,36 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>168</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>52</v>
+      <c r="A17" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1445,35 +1476,35 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="A18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -1482,16 +1513,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -1500,34 +1531,34 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
+        <v>67</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -1536,16 +1567,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1554,16 +1585,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -1572,16 +1603,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1590,16 +1621,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -1608,16 +1639,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -1626,16 +1657,16 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1644,16 +1675,16 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -1662,16 +1693,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>89</v>
+        <v>161</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>90</v>
+        <v>162</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1680,16 +1711,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>161</v>
+        <v>92</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>162</v>
+        <v>93</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>163</v>
+        <v>94</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -1697,89 +1728,89 @@
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+      <c r="A32" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
+      <c r="A33" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+      <c r="A34" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
+      <c r="A35" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -1788,16 +1819,16 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>172</v>
+        <v>100</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -1806,57 +1837,111 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>115</v>
+        <v>169</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -1956,10 +2041,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,9 +2386,33 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>181</v>
+      </c>
+      <c r="B41" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2318,11 +2427,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A37" sqref="A37"/>
+      <selection pane="topRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2654,10 +2763,34 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>172</v>
+      </c>
+      <c r="B38" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>181</v>
+      </c>
+      <c r="B39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>182</v>
+      </c>
+      <c r="B40" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>